<commit_message>
Fixed string connector ID bug
Signed-off-by: aytugy <aytug.yavuzer@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/external/utils/aggregator_info.xlsx
+++ b/external/utils/aggregator_info.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egu\PycharmProjects\FLOW\sogno_services\evrich_citl\external\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aytugy\Desktop\workspace\evrich\external\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE757B0F-13C0-4B77-B276-A02A6A09A611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="socket_info" sheetId="13" r:id="rId1"/>
     <sheet name="1" sheetId="9" r:id="rId2"/>
     <sheet name="2" sheetId="4" r:id="rId3"/>
     <sheet name="3" sheetId="11" r:id="rId4"/>
-    <sheet name="4" sheetId="14" r:id="rId5"/>
-    <sheet name="5" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>cu_id</t>
   </si>
@@ -75,12 +74,18 @@
   </si>
   <si>
     <t>CC03_c</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -136,9 +141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -176,9 +181,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,7 +253,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,14 +426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B90A685-6DE2-42D0-8D24-8AE5CC965569}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -442,8 +447,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -464,8 +469,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -494,61 +499,6 @@
       </c>
       <c r="C6">
         <v>9005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>9006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>9007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>9008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>9009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>9010</v>
       </c>
     </row>
   </sheetData>
@@ -558,14 +508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -633,14 +583,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -707,14 +657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -778,30 +728,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>